<commit_message>
updated chaining of login
</commit_message>
<xml_diff>
--- a/7rMart_Project/src/test/resources/testdata.xlsx
+++ b/7rMart_Project/src/test/resources/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devika\eclipse-workspace\GroceryApp\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devika\git\7rmartproject\7rMart_Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22B63BF-DA3D-48A3-B7AD-9B1A203C088B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CEFB11-6442-4F92-A854-5B3C0ECC537E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>News</t>
   </si>
   <si>
-    <t>news headlines sports news</t>
-  </si>
-  <si>
     <t>Obsqura automation Project started</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>Washing Machine</t>
+  </si>
+  <si>
+    <t>Obsqura automation Project completed</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -667,18 +667,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -690,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103CFEC1-02F4-4443-9E4A-3AE7D98D9972}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -703,10 +703,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -714,10 +714,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -849,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9932CCCB-60FD-49A6-BB66-E3D3889BAF26}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +865,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>